<commit_message>
Creación de question para la transacción
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/tarjetacredito/TarjetaCreditoNoPropia.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/tarjetacredito/TarjetaCreditoNoPropia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\tarjetacredito\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047A43EA-D09C-456E-B9E1-9D50BFC3CB7C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FC64A5-793B-4C36-B496-2CE39474ED2B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -155,6 +155,15 @@
   </si>
   <si>
     <t>Dólares</t>
+  </si>
+  <si>
+    <t>5326666666666666</t>
+  </si>
+  <si>
+    <t>Pago total en dólares</t>
+  </si>
+  <si>
+    <t>Pago total en pesos</t>
   </si>
 </sst>
 </file>
@@ -242,13 +251,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -560,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -641,23 +649,23 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="11" customFormat="1">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:20" s="10" customFormat="1">
+      <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -672,54 +680,54 @@
       <c r="J2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="Q2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="R2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="S2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="T2" s="11" t="s">
+      <c r="T2" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="11" customFormat="1">
-      <c r="A3" s="9">
+    <row r="3" spans="1:20" s="10" customFormat="1">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -734,54 +742,54 @@
       <c r="J3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="P3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="Q3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="R3" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="S3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="T3" s="11" t="s">
+      <c r="T3" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -796,42 +804,54 @@
       <c r="J4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="N4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="7"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
+      <c r="O4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -846,27 +866,36 @@
       <c r="J5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="M5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O5" s="7"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="M13" s="5"/>
+      <c r="O5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="T5" s="10" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Estabilizacion de la transacción
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/tarjetacredito/TarjetaCreditoNoPropia.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/tarjetacredito/TarjetaCreditoNoPropia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\tarjetacredito\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1C1857-4246-462B-BB48-674B7E8B2AE7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D38FB60-4073-4B68-BBC4-27DCA16730E1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,9 +67,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>1010111</t>
-  </si>
-  <si>
     <t>4321</t>
   </si>
   <si>
@@ -130,15 +127,9 @@
     <t>Pago mínimo en pesos</t>
   </si>
   <si>
-    <t>406-132280-01</t>
-  </si>
-  <si>
     <t>0,00</t>
   </si>
   <si>
-    <t>userrobot2</t>
-  </si>
-  <si>
     <t>moneda</t>
   </si>
   <si>
@@ -164,18 +155,34 @@
   </si>
   <si>
     <t>80000</t>
+  </si>
+  <si>
+    <t>22493944</t>
+  </si>
+  <si>
+    <t>userrobot1</t>
+  </si>
+  <si>
+    <t>406-139440-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -191,6 +198,12 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -249,20 +262,22 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -570,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -633,273 +648,274 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="10" customFormat="1">
       <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>15</v>
+      <c r="B2" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>38</v>
+      <c r="D2" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="O2" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="12" t="s">
         <v>47</v>
-      </c>
-      <c r="R2" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="10" customFormat="1">
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>15</v>
+      <c r="B3" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" s="6" t="s">
+      <c r="P3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="P3" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="S3" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="T3" s="10" t="s">
-        <v>36</v>
+        <v>29</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>38</v>
+      <c r="D4" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="H4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="O4" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="Q4" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="R4" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="T4" s="10" t="s">
-        <v>36</v>
+        <v>29</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>15</v>
+        <v>28</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>38</v>
+      <c r="D5" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="N5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="O5" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="P5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="R5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="R5" s="10" t="s">
-        <v>40</v>
-      </c>
       <c r="S5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="T5" s="10" t="s">
-        <v>36</v>
+        <v>29</v>
+      </c>
+      <c r="T5" s="12" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="N3" r:id="rId2" xr:uid="{9C71363A-8202-4229-9AF8-9716E8F6F072}"/>

</xml_diff>